<commit_message>
BOM adjusted to numbers agreed with BB,ready to order
</commit_message>
<xml_diff>
--- a/design/BOM.xlsx
+++ b/design/BOM.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">CO2-Sensor</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
+    <t xml:space="preserve">7</t>
   </si>
   <si>
     <t xml:space="preserve">29.90</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Lora Antennenkabel</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">6.50</t>
@@ -213,7 +213,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,6 +247,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,10 +335,13 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -372,7 +379,7 @@
       </c>
       <c r="D3" s="5" t="n">
         <f aca="false">B3*C3</f>
-        <v>149.5</v>
+        <v>209.3</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>9</v>
@@ -390,7 +397,7 @@
       </c>
       <c r="D4" s="7" t="n">
         <f aca="false">B4*C4</f>
-        <v>47</v>
+        <v>65.8</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
@@ -408,7 +415,7 @@
       </c>
       <c r="D5" s="7" t="n">
         <f aca="false">B5*C5</f>
-        <v>132.5</v>
+        <v>185.5</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>15</v>
@@ -426,19 +433,19 @@
       </c>
       <c r="D6" s="8" t="n">
         <f aca="false">B6*C6</f>
-        <v>6.5</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="9" t="n">
         <f aca="false">SUM(D3:D6)</f>
-        <v>335.5</v>
+        <v>473.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>